<commit_message>
Dinh dang lai van ban
</commit_message>
<xml_diff>
--- a/TaiLieu/KeHoach.xlsx
+++ b/TaiLieu/KeHoach.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDED73C4-87AD-493C-B83C-9B0E639C7647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ke hoach thuc hien" sheetId="3" r:id="rId1"/>
@@ -19,8 +20,14 @@
     <definedName name="PeriodInPlan">#REF!=MEDIAN(#REF!,#REF!,#REF!+#REF!-1)</definedName>
     <definedName name="Plan">PeriodInPlan*(#REF!&gt;0)</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -117,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
@@ -435,17 +442,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Activity" xfId="2"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Project Headers" xfId="4"/>
-    <cellStyle name="Style 1" xfId="8"/>
-    <cellStyle name="Style 2" xfId="9"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Style 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Style 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -696,10 +703,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>

</xml_diff>